<commit_message>
added support for configuration files detecting in getdata and report sections, unconditional looping over data and generating results
</commit_message>
<xml_diff>
--- a/dell/2018-12-6_85625_export.xml_report.xlsx
+++ b/dell/2018-12-6_85625_export.xml_report.xlsx
@@ -11,6 +11,14 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>error: unsupported file:c:\gitrep\xmlparse\dell\2018-12-6_85625_export.xml</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -345,7 +353,16 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="74.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>